<commit_message>
New Outlier Thresh and Variance Figure
Very Pretty GGPlot version of the variance figure that prints properly! Horray!
Setting outlier threshold to 5 instead of 3 sd above the mean
</commit_message>
<xml_diff>
--- a/Data/OutputtedData/GWASPoly/WSMDP_Carb_GWASpoly_SeqG_NFBlup_EndoFixedEffect_FDRThresh_AllCarbWCandidateGenes.xlsx
+++ b/Data/OutputtedData/GWASPoly/WSMDP_Carb_GWASpoly_SeqG_NFBlup_EndoFixedEffect_FDRThresh_AllCarbWCandidateGenes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LHislop\Documents\GitHub\WSMDP_Carb\Data\OutputtedData\GWASPoly\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF97CEC0-3921-48FB-954D-49573225EA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52DC078-3665-433E-BB9D-F2CBA47C77F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7872" yWindow="192" windowWidth="17280" windowHeight="8964" xr2:uid="{F334FD38-1778-4852-A9B1-F7445D890BCA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F334FD38-1778-4852-A9B1-F7445D890BCA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -746,13 +746,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BECAB8B8-A43B-4124-BBAC-25F835C247F1}">
   <dimension ref="A1:X129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30:H30"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30:B129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
     <col min="7" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.33203125" customWidth="1"/>
     <col min="11" max="11" width="5.21875" customWidth="1"/>

</xml_diff>